<commit_message>
broke external link in spreadsheet / removed todos
</commit_message>
<xml_diff>
--- a/capacity-planning-template.xlsx
+++ b/capacity-planning-template.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NeilSmyth\Documents\dev-alkemio\github-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83377465-330F-47D5-AB7F-90958ADE273F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD01501E-05AD-48D9-AA65-44FC87DC3A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4240" windowWidth="14220" windowHeight="7200" activeTab="1" xr2:uid="{803F6BCA-D7A7-4AC9-BDD8-7DDDBA99C8E3}"/>
+    <workbookView xWindow="410" yWindow="350" windowWidth="9470" windowHeight="4970" activeTab="2" xr2:uid="{803F6BCA-D7A7-4AC9-BDD8-7DDDBA99C8E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Capacity" sheetId="2" r:id="rId2"/>
     <sheet name="GITHUB_EPICS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="EPICS_ESTIMATES">Table2[Estimate - Remaining]</definedName>
     <definedName name="EPICS_PERIOD">Table2[Period]</definedName>
@@ -84,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Capacity planning for Alkemio</t>
   </si>
@@ -135,19 +132,6 @@
   </si>
   <si>
     <t>Available</t>
-  </si>
-  <si>
-    <t>Filter criteria: 
-- repo: Alkemio
-- label: Epic
-- pipeline: Not closed</t>
-  </si>
-  <si>
-    <t>TBD
-- Use labels for initiatives?
-- Resource type breakdown per Epic
-- Make use of backlog ranking? + where?
-- Plan per team or in aggregate?</t>
   </si>
   <si>
     <t>ID</t>
@@ -648,45 +632,39 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>'[1]Capacity + Allocation'!$A$4:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2023 Q1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2023 Q2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2023 H2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2024</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>2023 Q1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2023 Q2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2023 H2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2024</c:v>
+              </c:pt>
+            </c:strLit>
           </c:cat>
           <c:val>
-            <c:numRef>
-              <c:f>'[1]Capacity + Allocation'!$B$4:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>400</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>260</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>500</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>0</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>400</c:v>
+              </c:pt>
+            </c:numLit>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -698,15 +676,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'[1]Capacity + Allocation'!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Available</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Available</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -780,45 +750,39 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>'[1]Capacity + Allocation'!$A$4:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2023 Q1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2023 Q2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2023 H2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2024</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>2023 Q1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2023 Q2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2023 H2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2024</c:v>
+              </c:pt>
+            </c:strLit>
           </c:cat>
           <c:val>
-            <c:numRef>
-              <c:f>'[1]Capacity + Allocation'!$C$4:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>600</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>500</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>100</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>300</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>600</c:v>
+              </c:pt>
+            </c:numLit>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1643,80 +1607,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Parameters"/>
-      <sheetName val="Capacity + Allocation"/>
-      <sheetName val="EPICS_GITHUB"/>
-      <sheetName val="VSTS_ValidationWS_1"/>
-      <sheetName val="capacity-planning-template_old"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="C3" t="str">
-            <v>Available</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>2023 Q1</v>
-          </cell>
-          <cell r="B4">
-            <v>260</v>
-          </cell>
-          <cell r="C4">
-            <v>500</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>2023 Q2</v>
-          </cell>
-          <cell r="B5">
-            <v>500</v>
-          </cell>
-          <cell r="C5">
-            <v>100</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>2023 H2</v>
-          </cell>
-          <cell r="B6">
-            <v>0</v>
-          </cell>
-          <cell r="C6">
-            <v>300</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>2024</v>
-          </cell>
-          <cell r="B7">
-            <v>400</v>
-          </cell>
-          <cell r="C7">
-            <v>600</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2053,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C4E8DA-25C2-4D1B-ADAA-0D2EA9E9D227}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showFormulas="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2247,7 +2137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF7D0EA-634C-4549-AD9B-059907E012FB}">
   <dimension ref="A4:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2325,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B334613F-B4E1-4A20-853A-4E00A027C2F3}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2343,13 +2233,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
-        <v>17</v>
-      </c>
+      <c r="A1" s="21"/>
       <c r="B1" s="21"/>
-      <c r="E1" s="22" t="s">
-        <v>18</v>
-      </c>
+      <c r="E1" s="22"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
@@ -2360,34 +2246,34 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -2395,16 +2281,16 @@
         <v>2447</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>11</v>
@@ -2414,7 +2300,7 @@
         <v>260</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -2422,16 +2308,16 @@
         <v>2332</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>12</v>
@@ -2441,7 +2327,7 @@
         <v>500</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -2449,16 +2335,16 @@
         <v>2222</v>
       </c>
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
       </c>
       <c r="F6" s="13">
         <v>2024</v>
@@ -2468,7 +2354,7 @@
         <v>400</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated to have Q1 + Q2 2024 setup
</commit_message>
<xml_diff>
--- a/capacity-planning-template.xlsx
+++ b/capacity-planning-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neil\Documents\dev-alkemio\github-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9D5ED0-E70D-40C6-A1C4-4D96031E3035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1029CF8E-39B7-4460-9E01-FF762E78EA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,13 @@
     <sheet name="GITHUB_EPICS" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">GITHUB_EPICS!$A$1:$L$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">GITHUB_EPICS!$A$1:$L$157</definedName>
     <definedName name="EPICS_ESTIMATE">GITHUB_EPICS!$F$2:$F$199</definedName>
     <definedName name="EPICS_PERIOD">GITHUB_EPICS!$G$2:$G$199</definedName>
     <definedName name="EPICS_STATUS">GITHUB_EPICS!$D$2:$D$199</definedName>
     <definedName name="EPICS_TYPE">GITHUB_EPICS!$E$2:$E$199</definedName>
-    <definedName name="PERIODS">Parameters!$A$6:$A$44</definedName>
-    <definedName name="PLANNING">Parameters!$A$6:$J$10</definedName>
+    <definedName name="PERIODS">Parameters!$A$6:$A$46</definedName>
+    <definedName name="PLANNING">Parameters!$A$6:$J$12</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="283">
   <si>
     <t>Capacity planning for Alkemio</t>
   </si>
@@ -352,9 +352,6 @@
     <t>Landing page: refinements + maintainability</t>
   </si>
   <si>
-    <t>QA Test suites catchup</t>
-  </si>
-  <si>
     <t>Notifications dashboard</t>
   </si>
   <si>
@@ -364,9 +361,6 @@
     <t>Operations: Platform monitoring</t>
   </si>
   <si>
-    <t>Reporting: Platform usage insights</t>
-  </si>
-  <si>
     <t>Data Integrity: v2</t>
   </si>
   <si>
@@ -580,9 +574,6 @@
     <t>I: Analytics via connectivity graph v1</t>
   </si>
   <si>
-    <t>Platform navigation</t>
-  </si>
-  <si>
     <t>I: Journey structure refresh</t>
   </si>
   <si>
@@ -661,18 +652,12 @@
     <t>Usage of Alkemio platform identities for Matrix</t>
   </si>
   <si>
-    <t>Innovation Library for users</t>
-  </si>
-  <si>
     <t>Analytics + monitoring: Dedicated elastic cluster</t>
   </si>
   <si>
     <t>Note: update to have each period start / end adjustable</t>
   </si>
   <si>
-    <t>2023-05-23</t>
-  </si>
-  <si>
     <t>2023-06-06</t>
   </si>
   <si>
@@ -694,9 +679,6 @@
     <t>Refresh preferences for notifications</t>
   </si>
   <si>
-    <t>Generative AI first use case</t>
-  </si>
-  <si>
     <t>Time Period Start</t>
   </si>
   <si>
@@ -721,12 +703,6 @@
     <t>TNO, UWV</t>
   </si>
   <si>
-    <t>2023-07-04</t>
-  </si>
-  <si>
-    <t>DSIH</t>
-  </si>
-  <si>
     <t>Sharing metrics of Space activity with leads</t>
   </si>
   <si>
@@ -739,9 +715,6 @@
     <t>I: Innovation Hubs</t>
   </si>
   <si>
-    <t>Client: Direct entity access</t>
-  </si>
-  <si>
     <t>Update of Journey settings tab: v1</t>
   </si>
   <si>
@@ -814,16 +787,115 @@
     <t>TIP, UWV</t>
   </si>
   <si>
-    <t>Reporting: sharing of reports, additional reports</t>
-  </si>
-  <si>
     <t>Innovation Flow: Definition to include goal/checklist/callouts</t>
   </si>
   <si>
     <t>Community: Multiple Lead Organizations on Space, Admin as Role</t>
   </si>
   <si>
-    <t>Client: Reduce client load times</t>
+    <t xml:space="preserve">QA: Improved Test Infrastructure </t>
+  </si>
+  <si>
+    <t>Reporting: Additional extensions</t>
+  </si>
+  <si>
+    <t>Spaces central + jobs to be done</t>
+  </si>
+  <si>
+    <t>2023-09-12</t>
+  </si>
+  <si>
+    <t>InnovationFlow Templates</t>
+  </si>
+  <si>
+    <t>UWV, Digicampus, Novum, VNG</t>
+  </si>
+  <si>
+    <t>Generative AI: guidance demonstrator</t>
+  </si>
+  <si>
+    <t>2023-08-01</t>
+  </si>
+  <si>
+    <t>2023-08-29</t>
+  </si>
+  <si>
+    <t>Epic,Product Discussion,Refinement</t>
+  </si>
+  <si>
+    <t>Client: Simplified logic via streamlined server api</t>
+  </si>
+  <si>
+    <t>2023-08-15</t>
+  </si>
+  <si>
+    <t>Svetoslav Petkov,user</t>
+  </si>
+  <si>
+    <t>Epic,Roadmap Discussion,Product Discussion</t>
+  </si>
+  <si>
+    <t>Defined</t>
+  </si>
+  <si>
+    <t>UWV, VNG, Digicampus</t>
+  </si>
+  <si>
+    <t>2023-09-26</t>
+  </si>
+  <si>
+    <t>Guidance: general availability</t>
+  </si>
+  <si>
+    <t>Reporting: (automated) sharing of reports , read only access</t>
+  </si>
+  <si>
+    <t>Client: Optimize user responsiveness</t>
+  </si>
+  <si>
+    <t>Callout type: Poll</t>
+  </si>
+  <si>
+    <t>VNG, Data Autonomy</t>
+  </si>
+  <si>
+    <t>Default callouts extended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guidance: beta testing with Alkemio community </t>
+  </si>
+  <si>
+    <t>Switch to Vite from Webpack</t>
+  </si>
+  <si>
+    <t>Client: Technical debt, responsiveness</t>
+  </si>
+  <si>
+    <t>Callout templates</t>
+  </si>
+  <si>
+    <t>Community Invitations: Allowing inviting many (external) users at once</t>
+  </si>
+  <si>
+    <t>Callouts UX refinements</t>
+  </si>
+  <si>
+    <t>Callouts: refreshed create flow</t>
+  </si>
+  <si>
+    <t>Journey settings v2: Space platform info, challenge, opportunity</t>
+  </si>
+  <si>
+    <t>Community refinements: challenge invitations,  membership policy</t>
+  </si>
+  <si>
+    <t>2024 Q1</t>
+  </si>
+  <si>
+    <t>2024 Q2</t>
+  </si>
+  <si>
+    <t>2024 H2</t>
   </si>
 </sst>
 </file>
@@ -940,7 +1012,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -970,6 +1042,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in 20% - Accent6" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1204,9 +1278,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Capacity!$A$5:$A$9</c:f>
+              <c:f>Capacity!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2023 Q1</c:v>
                 </c:pt>
@@ -1220,30 +1294,42 @@
                   <c:v>2023 Q4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2024</c:v>
+                  <c:v>2024 Q1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2024 Q2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2024 H2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Capacity!$B$5:$B$9</c:f>
+              <c:f>Capacity!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>340</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>950</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>530</c:v>
+                  <c:v>1010</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1315,9 +1401,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Capacity!$A$5:$A$9</c:f>
+              <c:f>Capacity!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2023 Q1</c:v>
                 </c:pt>
@@ -1331,17 +1417,23 @@
                   <c:v>2023 Q4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2024</c:v>
+                  <c:v>2024 Q1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2024 Q2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2024 H2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Capacity!$C$5:$C$9</c:f>
+              <c:f>Capacity!$C$5:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1349,13 +1441,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>720</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>650</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>2607.1428571428573</c:v>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1307.1428571428571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1623,10 +1721,10 @@
                   <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1697,7 +1795,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1836,10 +1934,10 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>170</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>170</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1909,10 +2007,10 @@
                   <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>310</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2050,13 +2148,13 @@
                   <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>360</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>110</c:v>
+                  <c:v>290</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2126,10 +2224,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2887,14 +2985,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>151562</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>26770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2923,13 +3021,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1200150</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>155574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2959,8 +3057,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A4:M9" totalsRowShown="0">
-  <autoFilter ref="A4:M9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A4:M11" totalsRowShown="0">
+  <autoFilter ref="A4:M11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Delivery"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Planned" dataDxfId="7">
@@ -3301,10 +3399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3339,7 +3437,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>3</v>
@@ -3351,10 +3449,10 @@
         <v>5</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>6</v>
@@ -3426,26 +3524,26 @@
         <v>0.8</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" ref="E7:E10" si="0">(C7-B7)/7/2</f>
+        <f t="shared" ref="E7:E12" si="0">(C7-B7)/7/2</f>
         <v>6</v>
       </c>
       <c r="F7" s="6">
         <v>6</v>
       </c>
       <c r="G7" s="6">
-        <f t="shared" ref="G7:G10" si="1">E7-F7</f>
+        <f t="shared" ref="G7:G12" si="1">E7-F7</f>
         <v>0</v>
       </c>
       <c r="H7" s="7">
         <v>200</v>
       </c>
       <c r="I7" s="7">
-        <f t="shared" ref="I7:I10" si="2">H7*G7*D7</f>
+        <f t="shared" ref="I7:I12" si="2">H7*G7*D7</f>
         <v>0</v>
       </c>
       <c r="J7" s="2"/>
       <c r="M7" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -3467,18 +3565,18 @@
         <v>7</v>
       </c>
       <c r="F8" s="6">
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="H8" s="7">
         <v>200</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" si="2"/>
-        <v>720</v>
+        <v>180</v>
       </c>
       <c r="J8" s="2"/>
     </row>
@@ -3487,7 +3585,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="4">
-        <f t="shared" ref="B9:B10" si="3">C8</f>
+        <f t="shared" ref="B9" si="3">C8</f>
         <v>45194</v>
       </c>
       <c r="C9" s="4">
@@ -3517,36 +3615,104 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>2024</v>
+      <c r="A10" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="B10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B10:B11" si="4">C9</f>
         <v>45292</v>
       </c>
       <c r="C10" s="4">
-        <v>45657</v>
+        <v>45383</v>
       </c>
       <c r="D10" s="5">
         <v>0.5</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" si="0"/>
-        <v>26.071428571428573</v>
-      </c>
-      <c r="F10" s="6"/>
+        <f t="shared" ref="E10:E11" si="5">(C10-B10)/7/2</f>
+        <v>6.5</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.5</v>
+      </c>
       <c r="G10" s="6">
-        <f t="shared" si="1"/>
-        <v>26.071428571428573</v>
+        <f t="shared" ref="G10:G11" si="6">E10-F10</f>
+        <v>6</v>
       </c>
       <c r="H10" s="7">
         <v>200</v>
       </c>
       <c r="I10" s="7">
+        <f t="shared" ref="I10:I11" si="7">H10*G10*D10</f>
+        <v>600</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="4"/>
+        <v>45383</v>
+      </c>
+      <c r="C11" s="4">
+        <v>45474</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="5"/>
+        <v>6.5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="H11" s="7">
+        <v>200</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="7"/>
+        <v>600</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B12" s="4">
+        <f>C11</f>
+        <v>45474</v>
+      </c>
+      <c r="C12" s="4">
+        <v>45657</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>13.071428571428571</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6">
+        <f t="shared" si="1"/>
+        <v>13.071428571428571</v>
+      </c>
+      <c r="H12" s="7">
+        <v>200</v>
+      </c>
+      <c r="I12" s="7">
         <f t="shared" si="2"/>
-        <v>2607.1428571428573</v>
-      </c>
-      <c r="J10" s="2"/>
+        <v>1307.1428571428571</v>
+      </c>
+      <c r="J12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3569,10 +3735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A4:M9"/>
+  <dimension ref="A4:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3599,10 +3765,10 @@
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
         <v>40</v>
@@ -3614,7 +3780,7 @@
         <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K4" t="s">
         <v>81</v>
@@ -3685,7 +3851,7 @@
       </c>
       <c r="B6">
         <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A6, EPICS_STATUS, "&lt;&gt;Done")</f>
-        <v>340</v>
+        <v>130</v>
       </c>
       <c r="C6" s="9">
         <f>Parameters!I7</f>
@@ -3693,11 +3859,11 @@
       </c>
       <c r="D6">
         <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A6, EPICS_STATUS, "Done")</f>
-        <v>460</v>
+        <v>640</v>
       </c>
       <c r="E6" s="11">
         <f>SUM(Table3[[#This Row],[Done]], Table3[[#This Row],[Planned]])</f>
-        <v>800</v>
+        <v>770</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -3725,7 +3891,7 @@
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="M6">
         <f>Table3[[#This Row],[Total]]-SUM(F6:L6)</f>
@@ -3739,23 +3905,23 @@
       </c>
       <c r="B7">
         <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A7, EPICS_STATUS, "&lt;&gt;Done")</f>
-        <v>950</v>
+        <v>600</v>
       </c>
       <c r="C7" s="9">
         <f>Parameters!I8</f>
-        <v>720</v>
+        <v>180</v>
       </c>
       <c r="D7">
         <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A7, EPICS_STATUS, "Done")</f>
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="E7" s="11">
         <f>SUM(Table3[[#This Row],[Done]], Table3[[#This Row],[Planned]])</f>
-        <v>950</v>
+        <v>910</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -3767,11 +3933,11 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>240</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>310</v>
+        <v>230</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
@@ -3779,11 +3945,11 @@
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>360</v>
+        <v>230</v>
       </c>
       <c r="M7">
         <f>Table3[[#This Row],[Total]]-SUM(F7:L7)</f>
-        <v>0</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -3793,7 +3959,7 @@
       </c>
       <c r="B8">
         <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A8, EPICS_STATUS, "&lt;&gt;Done")</f>
-        <v>530</v>
+        <v>1010</v>
       </c>
       <c r="C8" s="9">
         <f>Parameters!I9</f>
@@ -3805,15 +3971,15 @@
       </c>
       <c r="E8" s="11">
         <f>SUM(Table3[[#This Row],[Done]], Table3[[#This Row],[Planned]])</f>
-        <v>530</v>
+        <v>1010</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
@@ -3821,11 +3987,11 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
@@ -3833,64 +3999,170 @@
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>290</v>
       </c>
       <c r="M8">
         <f>Table3[[#This Row],[Total]]-SUM(F8:L8)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
-        <f>Parameters!A10</f>
-        <v>2024</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="15">
         <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_STATUS, "&lt;&gt;Done")</f>
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <f>Parameters!I10</f>
-        <v>2607.1428571428573</v>
-      </c>
-      <c r="D9">
+        <v>600</v>
+      </c>
+      <c r="D9" s="15">
         <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_STATUS, "Done")</f>
         <v>0</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="16">
         <f>SUM(Table3[[#This Row],[Done]], Table3[[#This Row],[Planned]])</f>
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="15">
         <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_TYPE, F$4)</f>
         <v>0</v>
       </c>
-      <c r="G9">
-        <f t="shared" ref="G9:L9" si="1">SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_TYPE, G$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+      <c r="G9" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_TYPE, G$4, EPICS_STATUS, "&lt;&gt;Done")</f>
         <v>0</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_TYPE, H$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_TYPE, I$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_TYPE, J$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_TYPE, K$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A9, EPICS_TYPE, L$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="15">
+        <f>Table3[[#This Row],[Total]]-SUM(F9:L9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="9">
+        <f>Parameters!I10</f>
+        <v>600</v>
+      </c>
+      <c r="D10" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_STATUS, "Done")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
+        <f>SUM(Table3[[#This Row],[Done]], Table3[[#This Row],[Planned]])</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_TYPE, F$4)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_TYPE, G$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_TYPE, H$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_TYPE, I$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_TYPE, J$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_TYPE, K$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="15">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A10, EPICS_TYPE, L$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="15">
+        <f>Table3[[#This Row],[Total]]-SUM(F10:L10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="str">
+        <f>Parameters!A12</f>
+        <v>2024 H2</v>
+      </c>
+      <c r="B11">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A11, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>Parameters!I12</f>
+        <v>1307.1428571428571</v>
+      </c>
+      <c r="D11">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A11, EPICS_STATUS, "Done")</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <f>SUM(Table3[[#This Row],[Done]], Table3[[#This Row],[Planned]])</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A11, EPICS_TYPE, F$4)</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:L11" si="1">SUMIFS(EPICS_ESTIMATE, EPICS_PERIOD, $A11, EPICS_TYPE, G$4, EPICS_STATUS, "&lt;&gt;Done")</f>
+        <v>0</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J9">
+      <c r="J11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9">
+      <c r="K11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9">
+      <c r="L11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M9">
-        <f>Table3[[#This Row],[Total]]-SUM(F9:L9)</f>
+      <c r="M11">
+        <f>Table3[[#This Row],[Total]]-SUM(F11:L11)</f>
         <v>0</v>
       </c>
     </row>
@@ -3907,10 +4179,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51DC3D3-F51C-4A1C-8876-FB0FD1045D79}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3963,7 +4235,7 @@
         <v>21</v>
       </c>
       <c r="L1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
@@ -3974,7 +4246,7 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -3989,7 +4261,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I2">
         <v>20</v>
@@ -4009,7 +4281,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F3">
         <v>30</v>
@@ -4029,7 +4301,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
         <v>93</v>
@@ -4038,7 +4310,7 @@
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -4163,13 +4435,13 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F8">
         <v>50</v>
@@ -4181,7 +4453,7 @@
         <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
@@ -4198,7 +4470,7 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F9">
         <v>80</v>
@@ -4227,13 +4499,13 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -4259,7 +4531,7 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F11">
         <v>30</v>
@@ -4323,7 +4595,7 @@
         <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F13">
         <v>50</v>
@@ -4390,7 +4662,7 @@
         <v>34</v>
       </c>
       <c r="L15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
@@ -4407,7 +4679,7 @@
         <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F16">
         <v>30</v>
@@ -4424,7 +4696,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
         <v>88</v>
@@ -4442,7 +4714,7 @@
         <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I17">
         <v>30</v>
@@ -4465,7 +4737,7 @@
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -4474,7 +4746,7 @@
         <v>9</v>
       </c>
       <c r="H18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I18">
         <v>10</v>
@@ -4488,13 +4760,13 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D19" t="s">
         <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F19">
         <v>20</v>
@@ -4514,10 +4786,10 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
@@ -4531,13 +4803,13 @@
         <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D21" t="s">
         <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F21">
         <v>30</v>
@@ -4580,13 +4852,13 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F23">
         <v>50</v>
@@ -4603,10 +4875,10 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E24" t="s">
         <v>96</v>
@@ -4629,10 +4901,10 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E25" t="s">
         <v>96</v>
@@ -4655,19 +4927,19 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F26">
         <v>80</v>
       </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -4678,13 +4950,13 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F27">
         <v>50</v>
@@ -4698,39 +4970,39 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>143</v>
+        <v>224</v>
       </c>
       <c r="C28" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="D28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>80</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
       </c>
       <c r="G28" t="s">
         <v>56</v>
       </c>
+      <c r="K28" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
-      </c>
-      <c r="E29" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="G29" t="s">
         <v>56</v>
@@ -4741,19 +5013,16 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
-      </c>
-      <c r="F30">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G30" t="s">
         <v>56</v>
@@ -4761,22 +5030,22 @@
     </row>
     <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>139</v>
       </c>
       <c r="C31" t="s">
-        <v>241</v>
+        <v>134</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E31" t="s">
         <v>96</v>
       </c>
       <c r="F31">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G31" t="s">
         <v>56</v>
@@ -4787,40 +5056,43 @@
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="E32" t="s">
-        <v>80</v>
+        <v>110</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
       </c>
       <c r="G32" t="s">
         <v>56</v>
       </c>
-      <c r="K32" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D33" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="E33" t="s">
         <v>96</v>
       </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
       <c r="G33" t="s">
         <v>56</v>
       </c>
@@ -4830,16 +5102,16 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C34" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="F34">
         <v>30</v>
@@ -4847,8 +5119,14 @@
       <c r="G34" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>264</v>
+      </c>
+      <c r="J34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -4856,22 +5134,19 @@
         <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>245</v>
+        <v>152</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="E35" t="s">
         <v>80</v>
       </c>
-      <c r="F35">
-        <v>30</v>
-      </c>
       <c r="G35" t="s">
-        <v>55</v>
-      </c>
-      <c r="H35" t="s">
-        <v>221</v>
+        <v>56</v>
+      </c>
+      <c r="K35" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -4879,19 +5154,16 @@
         <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
-      </c>
-      <c r="F36">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="G36" t="s">
         <v>56</v>
@@ -4902,22 +5174,25 @@
         <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>238</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="F37">
         <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>247</v>
+        <v>56</v>
+      </c>
+      <c r="H37" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -4925,22 +5200,22 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>231</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F38">
         <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>247</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -4948,28 +5223,22 @@
         <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>214</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="F39">
         <v>50</v>
       </c>
       <c r="G39" t="s">
-        <v>247</v>
-      </c>
-      <c r="H39" t="s">
-        <v>94</v>
-      </c>
-      <c r="I39">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -4977,22 +5246,25 @@
         <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="F40">
         <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>247</v>
+        <v>56</v>
+      </c>
+      <c r="H40" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5000,16 +5272,22 @@
         <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>229</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>230</v>
       </c>
       <c r="D41" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="E41" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41">
+        <v>30</v>
       </c>
       <c r="G41" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5017,22 +5295,22 @@
         <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E42" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="F42">
         <v>30</v>
       </c>
       <c r="G42" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5043,22 +5321,25 @@
         <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>137</v>
+        <v>248</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>31</v>
       </c>
       <c r="E43" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="F43">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s">
-        <v>247</v>
-      </c>
-      <c r="K43" t="s">
-        <v>29</v>
+        <v>238</v>
+      </c>
+      <c r="H43" t="s">
+        <v>94</v>
+      </c>
+      <c r="I43">
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5066,22 +5347,25 @@
         <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" t="s">
         <v>130</v>
       </c>
-      <c r="D44" t="s">
-        <v>64</v>
-      </c>
       <c r="E44" t="s">
-        <v>112</v>
+        <v>81</v>
+      </c>
+      <c r="F44">
+        <v>30</v>
       </c>
       <c r="G44" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -5089,51 +5373,36 @@
         <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>172</v>
       </c>
       <c r="D45" t="s">
-        <v>41</v>
-      </c>
-      <c r="E45" t="s">
-        <v>80</v>
-      </c>
-      <c r="F45">
-        <v>80</v>
+        <v>153</v>
       </c>
       <c r="G45" t="s">
-        <v>55</v>
-      </c>
-      <c r="H45" t="s">
-        <v>221</v>
-      </c>
-      <c r="I45">
-        <v>20</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E46" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="F46">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G46" t="s">
-        <v>247</v>
-      </c>
-      <c r="J46" t="s">
-        <v>51</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5144,16 +5413,22 @@
         <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>109</v>
+      </c>
+      <c r="F47">
+        <v>30</v>
       </c>
       <c r="G47" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="K47" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5164,42 +5439,39 @@
         <v>36</v>
       </c>
       <c r="C48" t="s">
-        <v>227</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>64</v>
       </c>
       <c r="E48" t="s">
-        <v>80</v>
-      </c>
-      <c r="F48">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="G48" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
         <v>106</v>
       </c>
       <c r="D49" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E49" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F49">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G49" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="J49" t="s">
         <v>51</v>
@@ -5213,19 +5485,16 @@
         <v>26</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D50" t="s">
         <v>64</v>
       </c>
       <c r="E50" t="s">
-        <v>112</v>
-      </c>
-      <c r="F50">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="G50" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5233,22 +5502,22 @@
         <v>25</v>
       </c>
       <c r="B51" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>219</v>
       </c>
       <c r="D51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E51" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="F51">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G51" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5259,22 +5528,22 @@
         <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E52" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F52">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="G52" t="s">
-        <v>247</v>
-      </c>
-      <c r="K52" t="s">
-        <v>29</v>
+        <v>238</v>
+      </c>
+      <c r="J52" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5285,19 +5554,19 @@
         <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D53" t="s">
         <v>64</v>
       </c>
       <c r="E53" t="s">
-        <v>80</v>
+        <v>110</v>
+      </c>
+      <c r="F53">
+        <v>20</v>
       </c>
       <c r="G53" t="s">
-        <v>247</v>
-      </c>
-      <c r="K53" t="s">
-        <v>98</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5305,25 +5574,22 @@
         <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D54" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F54">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G54" t="s">
-        <v>247</v>
-      </c>
-      <c r="J54" t="s">
-        <v>37</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5334,19 +5600,22 @@
         <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D55" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E55" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F55">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="G55" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="K55" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5354,28 +5623,22 @@
         <v>25</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D56" t="s">
-        <v>132</v>
+        <v>64</v>
       </c>
       <c r="E56" t="s">
         <v>80</v>
       </c>
-      <c r="F56">
-        <v>30</v>
-      </c>
       <c r="G56" t="s">
-        <v>247</v>
-      </c>
-      <c r="J56" t="s">
-        <v>34</v>
+        <v>238</v>
       </c>
       <c r="K56" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5386,22 +5649,22 @@
         <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="E57" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F57">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G57" t="s">
-        <v>247</v>
-      </c>
-      <c r="K57" t="s">
-        <v>29</v>
+        <v>56</v>
+      </c>
+      <c r="J57" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5412,22 +5675,19 @@
         <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E58" t="s">
         <v>92</v>
       </c>
       <c r="F58">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G58" t="s">
-        <v>247</v>
-      </c>
-      <c r="J58" t="s">
-        <v>48</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5435,74 +5695,80 @@
         <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E59" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F59">
         <v>30</v>
       </c>
       <c r="G59" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="J59" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="K59" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C60" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
         <v>64</v>
       </c>
       <c r="E60" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F60">
         <v>20</v>
       </c>
       <c r="G60" t="s">
-        <v>247</v>
-      </c>
-      <c r="J60" t="s">
-        <v>51</v>
+        <v>238</v>
+      </c>
+      <c r="K60" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C61" t="s">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E61" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="F61">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G61" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="J61" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5510,80 +5776,74 @@
         <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E62" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="F62">
         <v>30</v>
       </c>
       <c r="G62" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="J62" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="D63" t="s">
-        <v>132</v>
+        <v>64</v>
       </c>
       <c r="E63" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="F63">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G63" t="s">
-        <v>247</v>
-      </c>
-      <c r="I63">
-        <v>10</v>
+        <v>238</v>
       </c>
       <c r="J63" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="D64" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="E64" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F64">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="G64" t="s">
-        <v>247</v>
-      </c>
-      <c r="J64" t="s">
-        <v>34</v>
-      </c>
-      <c r="K64" t="s">
-        <v>29</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5591,51 +5851,51 @@
         <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C65" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="D65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E65" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F65">
         <v>30</v>
       </c>
       <c r="G65" t="s">
-        <v>247</v>
-      </c>
-      <c r="J65" t="s">
-        <v>51</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E66" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F66">
         <v>30</v>
       </c>
       <c r="G66" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="I66">
+        <v>10</v>
       </c>
       <c r="J66" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5643,22 +5903,28 @@
         <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>26</v>
       </c>
       <c r="C67" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="D67" t="s">
-        <v>132</v>
+        <v>64</v>
       </c>
       <c r="E67" t="s">
         <v>80</v>
       </c>
       <c r="F67">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="G67" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="J67" t="s">
+        <v>34</v>
+      </c>
+      <c r="K67" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5666,45 +5932,51 @@
         <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
       <c r="C68" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="D68" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E68" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F68">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G68" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="J68" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
-        <v>167</v>
+        <v>72</v>
       </c>
       <c r="D69" t="s">
-        <v>155</v>
+        <v>130</v>
+      </c>
+      <c r="E69" t="s">
+        <v>92</v>
       </c>
       <c r="F69">
         <v>30</v>
       </c>
       <c r="G69" t="s">
-        <v>247</v>
-      </c>
-      <c r="K69" t="s">
-        <v>168</v>
+        <v>238</v>
+      </c>
+      <c r="J69" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5712,22 +5984,22 @@
         <v>25</v>
       </c>
       <c r="B70" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="C70" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="D70" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E70" t="s">
-        <v>111</v>
+        <v>80</v>
+      </c>
+      <c r="F70">
+        <v>20</v>
       </c>
       <c r="G70" t="s">
-        <v>247</v>
-      </c>
-      <c r="K70" t="s">
-        <v>29</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5735,25 +6007,25 @@
         <v>25</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="D71" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="E71" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F71">
-        <v>20</v>
-      </c>
-      <c r="J71" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="G71" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>25</v>
       </c>
@@ -5761,22 +6033,19 @@
         <v>26</v>
       </c>
       <c r="C72" t="s">
-        <v>230</v>
+        <v>165</v>
       </c>
       <c r="D72" t="s">
-        <v>41</v>
-      </c>
-      <c r="E72" t="s">
-        <v>96</v>
+        <v>153</v>
       </c>
       <c r="F72">
         <v>30</v>
       </c>
       <c r="G72" t="s">
-        <v>55</v>
-      </c>
-      <c r="H72" t="s">
-        <v>224</v>
+        <v>238</v>
+      </c>
+      <c r="K72" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5784,28 +6053,25 @@
         <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>26</v>
+        <v>141</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="D73" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="E73" t="s">
-        <v>96</v>
-      </c>
-      <c r="F73">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="G73" t="s">
-        <v>9</v>
-      </c>
-      <c r="H73" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+      <c r="K73" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>25</v>
       </c>
@@ -5813,7 +6079,7 @@
         <v>26</v>
       </c>
       <c r="C74" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D74" t="s">
         <v>41</v>
@@ -5822,16 +6088,10 @@
         <v>96</v>
       </c>
       <c r="F74">
-        <v>30</v>
-      </c>
-      <c r="G74" t="s">
-        <v>55</v>
-      </c>
-      <c r="H74" t="s">
-        <v>224</v>
-      </c>
-      <c r="I74">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="J74" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5839,22 +6099,25 @@
         <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C75" t="s">
-        <v>256</v>
+        <v>90</v>
       </c>
       <c r="D75" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="E75" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F75">
-        <v>80</v>
-      </c>
-      <c r="K75" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="G75" t="s">
+        <v>9</v>
+      </c>
+      <c r="H75" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5865,22 +6128,19 @@
         <v>36</v>
       </c>
       <c r="C76" t="s">
-        <v>113</v>
+        <v>246</v>
       </c>
       <c r="D76" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="E76" t="s">
         <v>80</v>
       </c>
       <c r="F76">
-        <v>50</v>
-      </c>
-      <c r="G76" t="s">
-        <v>10</v>
-      </c>
-      <c r="J76" t="s">
-        <v>34</v>
+        <v>80</v>
+      </c>
+      <c r="K76" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5888,16 +6148,16 @@
         <v>25</v>
       </c>
       <c r="B77" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C77" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
       <c r="D77" t="s">
         <v>28</v>
       </c>
       <c r="E77" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F77">
         <v>50</v>
@@ -5905,11 +6165,8 @@
       <c r="G77" t="s">
         <v>10</v>
       </c>
-      <c r="H77" t="s">
-        <v>208</v>
-      </c>
-      <c r="I77">
-        <v>15</v>
+      <c r="J77" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5920,28 +6177,25 @@
         <v>26</v>
       </c>
       <c r="C78" t="s">
-        <v>248</v>
+        <v>201</v>
       </c>
       <c r="D78" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E78" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="F78">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G78" t="s">
         <v>10</v>
       </c>
       <c r="H78" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="I78">
-        <v>30</v>
-      </c>
-      <c r="J78" t="s">
-        <v>209</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -5955,7 +6209,7 @@
         <v>83</v>
       </c>
       <c r="D79" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E79" t="s">
         <v>40</v>
@@ -5967,7 +6221,7 @@
         <v>10</v>
       </c>
       <c r="H79" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="I79">
         <v>30</v>
@@ -6071,7 +6325,7 @@
         <v>28</v>
       </c>
       <c r="E83" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F83">
         <v>30</v>
@@ -6091,10 +6345,10 @@
         <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D84" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E84" t="s">
         <v>80</v>
@@ -6134,16 +6388,16 @@
         <v>25</v>
       </c>
       <c r="B86" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C86" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D86" t="s">
         <v>28</v>
       </c>
       <c r="E86" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F86">
         <v>80</v>
@@ -6152,7 +6406,7 @@
         <v>10</v>
       </c>
       <c r="H86" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I86">
         <v>80</v>
@@ -6169,13 +6423,13 @@
         <v>26</v>
       </c>
       <c r="C87" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D87" t="s">
         <v>28</v>
       </c>
       <c r="E87" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F87">
         <v>20</v>
@@ -6184,7 +6438,7 @@
         <v>10</v>
       </c>
       <c r="H87" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6195,13 +6449,13 @@
         <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D88" t="s">
         <v>28</v>
       </c>
       <c r="E88" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F88">
         <v>30</v>
@@ -6210,10 +6464,10 @@
         <v>10</v>
       </c>
       <c r="H88" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K88" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6239,7 +6493,7 @@
         <v>10</v>
       </c>
       <c r="H89" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I89">
         <v>20</v>
@@ -6250,7 +6504,7 @@
     </row>
     <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B90" t="s">
         <v>26</v>
@@ -6271,7 +6525,7 @@
         <v>9</v>
       </c>
       <c r="H90" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I90">
         <v>10</v>
@@ -6291,7 +6545,7 @@
         <v>28</v>
       </c>
       <c r="E91" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F91">
         <v>80</v>
@@ -6308,28 +6562,13 @@
         <v>26</v>
       </c>
       <c r="C92" t="s">
-        <v>151</v>
+        <v>218</v>
       </c>
       <c r="D92" t="s">
-        <v>31</v>
-      </c>
-      <c r="E92" t="s">
-        <v>111</v>
-      </c>
-      <c r="F92">
-        <v>80</v>
-      </c>
-      <c r="G92" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" t="s">
-        <v>221</v>
-      </c>
-      <c r="I92">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="K92" t="s">
-        <v>223</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6337,31 +6576,13 @@
         <v>25</v>
       </c>
       <c r="B93" t="s">
-        <v>249</v>
+        <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>211</v>
+        <v>156</v>
       </c>
       <c r="D93" t="s">
-        <v>31</v>
-      </c>
-      <c r="E93" t="s">
-        <v>80</v>
-      </c>
-      <c r="F93">
-        <v>50</v>
-      </c>
-      <c r="G93" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" t="s">
-        <v>221</v>
-      </c>
-      <c r="I93">
-        <v>20</v>
-      </c>
-      <c r="K93" t="s">
-        <v>222</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6369,28 +6590,13 @@
         <v>25</v>
       </c>
       <c r="B94" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C94" t="s">
-        <v>204</v>
+        <v>157</v>
       </c>
       <c r="D94" t="s">
-        <v>28</v>
-      </c>
-      <c r="E94" t="s">
-        <v>80</v>
-      </c>
-      <c r="F94">
-        <v>30</v>
-      </c>
-      <c r="G94" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" t="s">
-        <v>207</v>
-      </c>
-      <c r="K94" t="s">
-        <v>225</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6398,16 +6604,19 @@
         <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="C95" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
       <c r="D95" t="s">
-        <v>155</v>
-      </c>
-      <c r="K95" t="s">
-        <v>29</v>
+        <v>153</v>
+      </c>
+      <c r="H95" t="s">
+        <v>94</v>
+      </c>
+      <c r="J95" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6415,243 +6624,237 @@
         <v>25</v>
       </c>
       <c r="B96" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="C96" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="D96" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>25</v>
       </c>
       <c r="B97" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="C97" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="D97" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="C98" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="D98" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>25</v>
       </c>
       <c r="B99" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="C99" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D99" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>25</v>
       </c>
       <c r="B100" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C100" t="s">
-        <v>178</v>
+        <v>221</v>
       </c>
       <c r="D100" t="s">
-        <v>155</v>
-      </c>
-      <c r="H100" t="s">
-        <v>94</v>
-      </c>
-      <c r="J100" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>25</v>
       </c>
       <c r="B101" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C101" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D101" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>25</v>
       </c>
       <c r="B102" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C102" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D102" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>25</v>
       </c>
       <c r="B103" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C103" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D103" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>25</v>
       </c>
       <c r="B104" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C104" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D104" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>25</v>
       </c>
       <c r="B105" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C105" t="s">
-        <v>229</v>
+        <v>185</v>
       </c>
       <c r="D105" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>25</v>
       </c>
       <c r="B106" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C106" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D106" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>25</v>
       </c>
       <c r="B107" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C107" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D107" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>25</v>
       </c>
       <c r="B108" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C108" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D108" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>25</v>
       </c>
       <c r="B109" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C109" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D109" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>25</v>
       </c>
       <c r="B110" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="C110" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D110" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>25</v>
       </c>
       <c r="B111" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C111" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D111" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>25</v>
       </c>
       <c r="B112" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C112" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D112" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6659,13 +6862,16 @@
         <v>25</v>
       </c>
       <c r="B113" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C113" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D113" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="G113" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6673,13 +6879,16 @@
         <v>25</v>
       </c>
       <c r="B114" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C114" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D114" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="G114" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6687,13 +6896,16 @@
         <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C115" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D115" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="G115" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6701,13 +6913,16 @@
         <v>25</v>
       </c>
       <c r="B116" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C116" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D116" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="G116" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6715,13 +6930,16 @@
         <v>25</v>
       </c>
       <c r="B117" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C117" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D117" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="G117" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6729,16 +6947,16 @@
         <v>25</v>
       </c>
       <c r="B118" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C118" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D118" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G118" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6746,16 +6964,16 @@
         <v>25</v>
       </c>
       <c r="B119" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C119" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D119" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G119" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6763,50 +6981,86 @@
         <v>25</v>
       </c>
       <c r="B120" t="s">
-        <v>175</v>
+        <v>26</v>
       </c>
       <c r="C120" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
       <c r="D120" t="s">
-        <v>155</v>
+        <v>43</v>
+      </c>
+      <c r="F120">
+        <v>50</v>
       </c>
       <c r="G120" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="H120" t="s">
+        <v>251</v>
+      </c>
+      <c r="K120" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>25</v>
       </c>
       <c r="B121" t="s">
-        <v>175</v>
+        <v>243</v>
       </c>
       <c r="C121" t="s">
-        <v>199</v>
+        <v>233</v>
       </c>
       <c r="D121" t="s">
-        <v>155</v>
+        <v>41</v>
+      </c>
+      <c r="E121" t="s">
+        <v>110</v>
+      </c>
+      <c r="F121">
+        <v>50</v>
       </c>
       <c r="G121" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="H121" t="s">
+        <v>256</v>
+      </c>
+      <c r="I121">
+        <v>20</v>
+      </c>
+      <c r="K121" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>25</v>
       </c>
       <c r="B122" t="s">
-        <v>175</v>
+        <v>26</v>
       </c>
       <c r="C122" t="s">
-        <v>200</v>
+        <v>63</v>
       </c>
       <c r="D122" t="s">
-        <v>155</v>
+        <v>41</v>
+      </c>
+      <c r="E122" t="s">
+        <v>80</v>
+      </c>
+      <c r="F122">
+        <v>80</v>
       </c>
       <c r="G122" t="s">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="H122" t="s">
+        <v>259</v>
+      </c>
+      <c r="I122">
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -6814,33 +7068,54 @@
         <v>25</v>
       </c>
       <c r="B123" t="s">
-        <v>175</v>
+        <v>26</v>
       </c>
       <c r="C123" t="s">
-        <v>201</v>
+        <v>239</v>
       </c>
       <c r="D123" t="s">
-        <v>155</v>
+        <v>28</v>
+      </c>
+      <c r="E123" t="s">
+        <v>109</v>
+      </c>
+      <c r="F123">
+        <v>80</v>
       </c>
       <c r="G123" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="H123" t="s">
+        <v>241</v>
+      </c>
+      <c r="I123">
+        <v>30</v>
+      </c>
+      <c r="J123" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>25</v>
       </c>
       <c r="B124" t="s">
-        <v>175</v>
+        <v>26</v>
       </c>
       <c r="C124" t="s">
-        <v>202</v>
+        <v>101</v>
       </c>
       <c r="D124" t="s">
-        <v>155</v>
+        <v>43</v>
+      </c>
+      <c r="E124" t="s">
+        <v>110</v>
+      </c>
+      <c r="F124">
+        <v>50</v>
       </c>
       <c r="G124" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.35">
@@ -6848,16 +7123,16 @@
         <v>25</v>
       </c>
       <c r="B125" t="s">
-        <v>26</v>
+        <v>229</v>
       </c>
       <c r="C125" t="s">
-        <v>242</v>
+        <v>163</v>
       </c>
       <c r="D125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E125" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="F125">
         <v>50</v>
@@ -6866,13 +7141,10 @@
         <v>55</v>
       </c>
       <c r="H125" t="s">
-        <v>221</v>
-      </c>
-      <c r="I125">
-        <v>20</v>
+        <v>256</v>
       </c>
       <c r="K125" t="s">
-        <v>254</v>
+        <v>144</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.35">
@@ -6880,16 +7152,16 @@
         <v>25</v>
       </c>
       <c r="B126" t="s">
-        <v>166</v>
+        <v>26</v>
       </c>
       <c r="C126" t="s">
-        <v>246</v>
+        <v>61</v>
       </c>
       <c r="D126" t="s">
         <v>43</v>
       </c>
       <c r="E126" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F126">
         <v>50</v>
@@ -6898,7 +7170,10 @@
         <v>55</v>
       </c>
       <c r="H126" t="s">
-        <v>224</v>
+        <v>256</v>
+      </c>
+      <c r="J126" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.35">
@@ -6906,28 +7181,28 @@
         <v>25</v>
       </c>
       <c r="B127" t="s">
-        <v>252</v>
+        <v>141</v>
       </c>
       <c r="C127" t="s">
-        <v>253</v>
+        <v>169</v>
       </c>
       <c r="D127" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="E127" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="F127">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G127" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H127" t="s">
-        <v>224</v>
+        <v>256</v>
       </c>
       <c r="K127" t="s">
-        <v>145</v>
+        <v>82</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.35">
@@ -6935,28 +7210,28 @@
         <v>25</v>
       </c>
       <c r="B128" t="s">
-        <v>238</v>
+        <v>26</v>
       </c>
       <c r="C128" t="s">
-        <v>165</v>
+        <v>68</v>
       </c>
       <c r="D128" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="E128" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F128">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G128" t="s">
         <v>55</v>
       </c>
       <c r="H128" t="s">
-        <v>224</v>
-      </c>
-      <c r="K128" t="s">
-        <v>146</v>
+        <v>256</v>
+      </c>
+      <c r="J128" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.35">
@@ -6964,25 +7239,25 @@
         <v>25</v>
       </c>
       <c r="B129" t="s">
-        <v>143</v>
+        <v>261</v>
       </c>
       <c r="C129" t="s">
-        <v>213</v>
+        <v>274</v>
       </c>
       <c r="D129" t="s">
-        <v>43</v>
-      </c>
-      <c r="E129" t="s">
-        <v>111</v>
+        <v>262</v>
       </c>
       <c r="F129">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G129" t="s">
         <v>55</v>
       </c>
       <c r="H129" t="s">
-        <v>250</v>
+        <v>259</v>
+      </c>
+      <c r="K129" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.35">
@@ -6990,28 +7265,25 @@
         <v>25</v>
       </c>
       <c r="B130" t="s">
-        <v>219</v>
+        <v>164</v>
       </c>
       <c r="C130" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="D130" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E130" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="F130">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G130" t="s">
         <v>55</v>
       </c>
       <c r="H130" t="s">
-        <v>224</v>
-      </c>
-      <c r="K130" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.35">
@@ -7019,28 +7291,28 @@
         <v>25</v>
       </c>
       <c r="B131" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C131" t="s">
-        <v>61</v>
+        <v>247</v>
       </c>
       <c r="D131" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E131" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="F131">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G131" t="s">
         <v>55</v>
       </c>
       <c r="H131" t="s">
-        <v>250</v>
-      </c>
-      <c r="J131" t="s">
-        <v>51</v>
+        <v>241</v>
+      </c>
+      <c r="K131" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.35">
@@ -7048,54 +7320,57 @@
         <v>25</v>
       </c>
       <c r="B132" t="s">
-        <v>143</v>
+        <v>26</v>
       </c>
       <c r="C132" t="s">
-        <v>214</v>
+        <v>254</v>
       </c>
       <c r="D132" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E132" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="F132">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G132" t="s">
         <v>55</v>
       </c>
       <c r="H132" t="s">
-        <v>250</v>
-      </c>
-      <c r="J132" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>25</v>
       </c>
       <c r="B133" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="C133" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
       <c r="D133" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E133" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="F133">
+        <v>50</v>
+      </c>
+      <c r="G133" t="s">
+        <v>10</v>
+      </c>
+      <c r="H133" t="s">
+        <v>259</v>
+      </c>
+      <c r="I133">
         <v>20</v>
       </c>
-      <c r="G133" t="s">
-        <v>55</v>
-      </c>
       <c r="K133" t="s">
-        <v>29</v>
+        <v>216</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.35">
@@ -7103,16 +7378,16 @@
         <v>25</v>
       </c>
       <c r="B134" t="s">
-        <v>26</v>
+        <v>213</v>
       </c>
       <c r="C134" t="s">
-        <v>68</v>
+        <v>235</v>
       </c>
       <c r="D134" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="E134" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="F134">
         <v>30</v>
@@ -7121,36 +7396,42 @@
         <v>55</v>
       </c>
       <c r="H134" t="s">
-        <v>224</v>
-      </c>
-      <c r="J134" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+      <c r="K134" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>25</v>
       </c>
       <c r="B135" t="s">
-        <v>143</v>
+        <v>26</v>
       </c>
       <c r="C135" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D135" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="E135" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F135">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="G135" t="s">
-        <v>55</v>
+        <v>10</v>
+      </c>
+      <c r="H135" t="s">
+        <v>259</v>
+      </c>
+      <c r="I135">
+        <v>20</v>
       </c>
       <c r="K135" t="s">
-        <v>82</v>
+        <v>217</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.35">
@@ -7158,16 +7439,16 @@
         <v>25</v>
       </c>
       <c r="B136" t="s">
-        <v>143</v>
+        <v>26</v>
       </c>
       <c r="C136" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="D136" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="E136" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="F136">
         <v>80</v>
@@ -7175,22 +7456,31 @@
       <c r="G136" t="s">
         <v>55</v>
       </c>
+      <c r="H136" t="s">
+        <v>259</v>
+      </c>
+      <c r="I136">
+        <v>10</v>
+      </c>
+      <c r="J136" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>25</v>
       </c>
       <c r="B137" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
       <c r="C137" t="s">
-        <v>102</v>
+        <v>222</v>
       </c>
       <c r="D137" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="E137" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F137">
         <v>50</v>
@@ -7198,37 +7488,40 @@
       <c r="G137" t="s">
         <v>55</v>
       </c>
+      <c r="H137" t="s">
+        <v>259</v>
+      </c>
+      <c r="I137">
+        <v>20</v>
+      </c>
+      <c r="K137" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>25</v>
       </c>
       <c r="B138" t="s">
-        <v>138</v>
+        <v>26</v>
       </c>
       <c r="C138" t="s">
-        <v>231</v>
+        <v>270</v>
       </c>
       <c r="D138" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E138" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F138">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G138" t="s">
         <v>55</v>
       </c>
       <c r="H138" t="s">
-        <v>221</v>
-      </c>
-      <c r="I138">
-        <v>20</v>
-      </c>
-      <c r="K138" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
     </row>
     <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -7236,25 +7529,16 @@
         <v>25</v>
       </c>
       <c r="B139" t="s">
-        <v>26</v>
+        <v>229</v>
       </c>
       <c r="C139" t="s">
-        <v>157</v>
+        <v>265</v>
       </c>
       <c r="D139" t="s">
-        <v>132</v>
-      </c>
-      <c r="E139" t="s">
-        <v>96</v>
-      </c>
-      <c r="F139">
-        <v>20</v>
-      </c>
-      <c r="G139" t="s">
-        <v>56</v>
-      </c>
-      <c r="I139">
-        <v>10</v>
+        <v>153</v>
+      </c>
+      <c r="H139" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.35">
@@ -7262,28 +7546,28 @@
         <v>25</v>
       </c>
       <c r="B140" t="s">
-        <v>233</v>
+        <v>26</v>
       </c>
       <c r="C140" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="D140" t="s">
-        <v>155</v>
+        <v>31</v>
       </c>
       <c r="E140" t="s">
+        <v>96</v>
+      </c>
+      <c r="F140">
         <v>80</v>
-      </c>
-      <c r="F140">
-        <v>50</v>
       </c>
       <c r="G140" t="s">
         <v>55</v>
       </c>
-      <c r="K140" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H140" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>25</v>
       </c>
@@ -7291,19 +7575,22 @@
         <v>26</v>
       </c>
       <c r="C141" t="s">
-        <v>215</v>
+        <v>155</v>
       </c>
       <c r="D141" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="E141" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="F141">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G141" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="I141">
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
@@ -7314,13 +7601,13 @@
         <v>26</v>
       </c>
       <c r="C142" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D142" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E142" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F142">
         <v>80</v>
@@ -7329,24 +7616,24 @@
         <v>10</v>
       </c>
       <c r="H142" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="I142">
         <v>20</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>25</v>
       </c>
       <c r="B143" t="s">
-        <v>26</v>
+        <v>141</v>
       </c>
       <c r="C143" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="D143" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E143" t="s">
         <v>96</v>
@@ -7355,64 +7642,328 @@
         <v>30</v>
       </c>
       <c r="G143" t="s">
+        <v>56</v>
+      </c>
+      <c r="J143" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>25</v>
+      </c>
+      <c r="B144" t="s">
+        <v>26</v>
+      </c>
+      <c r="C144" t="s">
+        <v>272</v>
+      </c>
+      <c r="D144" t="s">
+        <v>31</v>
+      </c>
+      <c r="E144" t="s">
+        <v>81</v>
+      </c>
+      <c r="F144">
+        <v>50</v>
+      </c>
+      <c r="G144" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>25</v>
-      </c>
-      <c r="B144" t="s">
+      <c r="H144" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>25</v>
+      </c>
+      <c r="B145" t="s">
+        <v>141</v>
+      </c>
+      <c r="C145" t="s">
+        <v>268</v>
+      </c>
+      <c r="D145" t="s">
+        <v>153</v>
+      </c>
+      <c r="G145" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>25</v>
+      </c>
+      <c r="B146" t="s">
+        <v>141</v>
+      </c>
+      <c r="C146" t="s">
+        <v>205</v>
+      </c>
+      <c r="D146" t="s">
+        <v>130</v>
+      </c>
+      <c r="E146" t="s">
+        <v>110</v>
+      </c>
+      <c r="F146">
+        <v>80</v>
+      </c>
+      <c r="G146" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>25</v>
+      </c>
+      <c r="B147" t="s">
+        <v>229</v>
+      </c>
+      <c r="C147" t="s">
+        <v>275</v>
+      </c>
+      <c r="D147" t="s">
+        <v>153</v>
+      </c>
+      <c r="E147" t="s">
+        <v>109</v>
+      </c>
+      <c r="G147" t="s">
+        <v>56</v>
+      </c>
+      <c r="K147" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>25</v>
+      </c>
+      <c r="B148" t="s">
+        <v>26</v>
+      </c>
+      <c r="C148" t="s">
+        <v>227</v>
+      </c>
+      <c r="D148" t="s">
+        <v>153</v>
+      </c>
+      <c r="E148" t="s">
+        <v>96</v>
+      </c>
+      <c r="F148">
+        <v>30</v>
+      </c>
+      <c r="G148" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>25</v>
+      </c>
+      <c r="B149" t="s">
+        <v>141</v>
+      </c>
+      <c r="C149" t="s">
+        <v>267</v>
+      </c>
+      <c r="D149" t="s">
+        <v>153</v>
+      </c>
+      <c r="E149" t="s">
+        <v>110</v>
+      </c>
+      <c r="F149">
+        <v>50</v>
+      </c>
+      <c r="G149" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>25</v>
+      </c>
+      <c r="B150" t="s">
+        <v>141</v>
+      </c>
+      <c r="C150" t="s">
+        <v>271</v>
+      </c>
+      <c r="D150" t="s">
+        <v>153</v>
+      </c>
+      <c r="H150" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>25</v>
+      </c>
+      <c r="B151" t="s">
+        <v>26</v>
+      </c>
+      <c r="C151" t="s">
+        <v>276</v>
+      </c>
+      <c r="D151" t="s">
+        <v>153</v>
+      </c>
+      <c r="F151">
+        <v>30</v>
+      </c>
+      <c r="G151" t="s">
+        <v>55</v>
+      </c>
+      <c r="J151" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>25</v>
+      </c>
+      <c r="B152" t="s">
+        <v>26</v>
+      </c>
+      <c r="C152" t="s">
+        <v>273</v>
+      </c>
+      <c r="D152" t="s">
+        <v>153</v>
+      </c>
+      <c r="E152" t="s">
+        <v>40</v>
+      </c>
+      <c r="F152">
+        <v>50</v>
+      </c>
+      <c r="G152" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>25</v>
+      </c>
+      <c r="B153" t="s">
+        <v>36</v>
+      </c>
+      <c r="C153" t="s">
+        <v>277</v>
+      </c>
+      <c r="D153" t="s">
+        <v>153</v>
+      </c>
+      <c r="F153">
+        <v>30</v>
+      </c>
+      <c r="G153" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>25</v>
+      </c>
+      <c r="B154" t="s">
+        <v>257</v>
+      </c>
+      <c r="C154" t="s">
+        <v>244</v>
+      </c>
+      <c r="D154" t="s">
+        <v>43</v>
+      </c>
+      <c r="E154" t="s">
+        <v>80</v>
+      </c>
+      <c r="F154">
+        <v>50</v>
+      </c>
+      <c r="G154" t="s">
+        <v>56</v>
+      </c>
+      <c r="H154" t="s">
+        <v>256</v>
+      </c>
+      <c r="K154" t="s">
         <v>143</v>
       </c>
-      <c r="C144" t="s">
-        <v>255</v>
-      </c>
-      <c r="D144" t="s">
-        <v>155</v>
-      </c>
-      <c r="E144" t="s">
-        <v>96</v>
-      </c>
-      <c r="F144">
-        <v>30</v>
-      </c>
-      <c r="G144" t="s">
+    </row>
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>25</v>
+      </c>
+      <c r="B155" t="s">
+        <v>141</v>
+      </c>
+      <c r="C155" t="s">
+        <v>250</v>
+      </c>
+      <c r="D155" t="s">
+        <v>153</v>
+      </c>
+      <c r="E155" t="s">
+        <v>80</v>
+      </c>
+      <c r="F155">
+        <v>50</v>
+      </c>
+      <c r="G155" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
-        <v>25</v>
-      </c>
-      <c r="B145" t="s">
-        <v>143</v>
-      </c>
-      <c r="C145" t="s">
-        <v>258</v>
-      </c>
-      <c r="D145" t="s">
-        <v>155</v>
-      </c>
-      <c r="E145" t="s">
-        <v>81</v>
-      </c>
-      <c r="F145">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>25</v>
+      </c>
+      <c r="B156" t="s">
+        <v>26</v>
+      </c>
+      <c r="C156" t="s">
+        <v>278</v>
+      </c>
+      <c r="D156" t="s">
+        <v>153</v>
+      </c>
+      <c r="F156">
         <v>50</v>
       </c>
-      <c r="G145" t="s">
-        <v>55</v>
+      <c r="G156" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>25</v>
+      </c>
+      <c r="B157" t="s">
+        <v>141</v>
+      </c>
+      <c r="C157" t="s">
+        <v>279</v>
+      </c>
+      <c r="D157" t="s">
+        <v>153</v>
+      </c>
+      <c r="G157" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L145" xr:uid="{F51DC3D3-F51C-4A1C-8876-FB0FD1045D79}">
+  <autoFilter ref="A1:L157" xr:uid="{F51DC3D3-F51C-4A1C-8876-FB0FD1045D79}">
     <filterColumn colId="6">
       <filters>
         <filter val="2023 Q3"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:L145">
-      <sortCondition ref="D1:D145"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A121:L153">
+      <sortCondition ref="D1:D157"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>